<commit_message>
df_priv_vehicles is correctly created
</commit_message>
<xml_diff>
--- a/Archetypes/stats_trans.xlsx
+++ b/Archetypes/stats_trans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asier.divasson\Documents\GitHub\CogniCity\Archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6567ABAD-7E97-4206-829E-C39153BF191F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7675AED-FB11-41C8-A019-C269B05D6C51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8364" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
   <si>
     <t>item_1</t>
   </si>
@@ -43,7 +43,10 @@
     <t>f_arch_0</t>
   </si>
   <si>
-    <t>conb_public</t>
+    <t>conb_car</t>
+  </si>
+  <si>
+    <t>E_car</t>
   </si>
   <si>
     <t>f_arch_1</t>
@@ -428,16 +431,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F2" sqref="F2:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -481,10 +481,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -521,10 +521,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -541,7 +541,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -561,10 +561,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -581,7 +581,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -601,21 +601,181 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
         <v>99</v>
       </c>
     </row>

</xml_diff>